<commit_message>
Adding bulk upload chages based on user id
</commit_message>
<xml_diff>
--- a/src/main/resources/static/BulkUploadTemplate.xlsx
+++ b/src/main/resources/static/BulkUploadTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DMS_git\dms-document-management\dms-document-management\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ACBB6D0-59F4-44C1-A3F8-54D59BB27205}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84561D16-FD56-4B9E-B83F-4F9A341CB318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>File Name</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>Upload Document</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>Contract Name</t>
   </si>
 </sst>
 </file>
@@ -377,10 +383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:K1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -389,14 +395,16 @@
     <col min="2" max="2" width="8.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.90625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.08984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.6328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.08984375" customWidth="1"/>
+    <col min="6" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -410,18 +418,24 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>